<commit_message>
Added a pdf with more data
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
+++ b/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
@@ -2396,8 +2396,8 @@
   </sheetPr>
   <dimension ref="A1:IH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -25281,16 +25281,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25547,29 +25543,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
-    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
-    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25596,9 +25585,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
+    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
+    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
random commit to fix things
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
+++ b/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
@@ -2396,8 +2396,8 @@
   </sheetPr>
   <dimension ref="A1:IH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -25281,16 +25281,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25547,29 +25543,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
-    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
-    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25596,9 +25585,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
+    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
+    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Formatted and combined data into data.xlsx
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
+++ b/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofh-my.sharepoint.com/personal/jmfalou_cougarnet_uh_edu/Documents/~Computer Science/z. Hackathon Projects/HalfStackDevs_CodeRedGenesis/Data Sets (Excels)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51B9ED8-7976-43C0-97D0-B6B12375364C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B51B9ED8-7976-43C0-97D0-B6B12375364C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09AE733F-ADC2-472A-808E-152A604A3E06}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BCBE03FC-E12F-46D2-A4C4-0593A89EA39B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
   <si>
     <t>--</t>
   </si>
@@ -649,6 +649,48 @@
       <t>8</t>
     </r>
   </si>
+  <si>
+    <t>2022 Performance by Country 1</t>
+  </si>
+  <si>
+    <t>Operated Total 2,3</t>
+  </si>
+  <si>
+    <t>All Others 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CO2 from Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CO2 from Imported Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Methane (CO2e) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nitrous Oxide (CO2e) </t>
+  </si>
+  <si>
+    <t>Total Greenhouse Gas Intensity (kg CO2e/BOE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Non-Fresh Water Withdrawn (million cubic meters) 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Produced Water Recycle/Reuse (million cubic meters) 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Number of Spills &gt; 100 Barrels</t>
+  </si>
+  <si>
+    <t>Waste (tonnes) 7</t>
+  </si>
+  <si>
+    <t>GLOBAL WORKFORCE 8</t>
+  </si>
+  <si>
+    <t>Total Operated Production (MMBOE) 9</t>
+  </si>
 </sst>
 </file>
 
@@ -1089,11 +1131,11 @@
       <sheetName val="Net Production - Annual Report"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1">
         <row r="8">
           <cell r="J8">
             <v>2103551.1800000002</v>
@@ -1226,7 +1268,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5">
+      <sheetData sheetId="5" refreshError="1">
         <row r="39">
           <cell r="E39">
             <v>450.85447457999999</v>
@@ -1263,7 +1305,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6">
+      <sheetData sheetId="6" refreshError="1">
         <row r="8">
           <cell r="E8">
             <v>77.12</v>
@@ -1409,7 +1451,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7">
+      <sheetData sheetId="7" refreshError="1">
         <row r="8">
           <cell r="E8">
             <v>665.71</v>
@@ -1451,15 +1493,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8">
-        <row r="33">
-          <cell r="AB33">
-            <v>8231969.29742378</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1">
         <row r="8">
           <cell r="E8">
             <v>4.42</v>
@@ -1575,7 +1611,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11">
+      <sheetData sheetId="11" refreshError="1">
         <row r="8">
           <cell r="E8">
             <v>38.119999999999997</v>
@@ -1654,7 +1690,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12">
+      <sheetData sheetId="12" refreshError="1">
         <row r="38">
           <cell r="E38">
             <v>9190.26</v>
@@ -1734,27 +1770,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13">
-        <row r="26">
-          <cell r="N26">
-            <v>6.1269090356293056E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14">
-        <row r="9">
-          <cell r="H9">
-            <v>2.9602357515478624E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="70">
-          <cell r="H70">
-            <v>634.37</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1796,10 +1814,10 @@
       <sheetName val="Transformed Data"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1">
         <row r="141">
           <cell r="H141">
             <v>9500</v>
@@ -1861,10 +1879,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1">
         <row r="6">
           <cell r="E6">
             <v>6242</v>
@@ -2070,25 +2088,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2396,8 +2414,8 @@
   </sheetPr>
   <dimension ref="A1:IH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2919,7 +2937,9 @@
       <c r="J3" s="51"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -3165,7 +3185,9 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -3913,7 +3935,9 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -4155,14 +4179,28 @@
       <c r="J8" s="9"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="O8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -4889,7 +4927,9 @@
       <c r="J11" s="9"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -5399,7 +5439,9 @@
       <c r="J13" s="16"/>
       <c r="K13" s="14"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -5661,14 +5703,28 @@
       <c r="J14" s="16"/>
       <c r="K14" s="14"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="O14" s="4">
+        <v>6129.1431650302193</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3216.65688</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1093.52761317</v>
+      </c>
+      <c r="R14" s="4">
+        <v>2103.5511800000004</v>
+      </c>
+      <c r="S14" s="4">
+        <v>685.36830000000009</v>
+      </c>
+      <c r="T14" s="4">
+        <v>13228.247138200219</v>
+      </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
@@ -5925,14 +5981,28 @@
       <c r="J15" s="16"/>
       <c r="K15" s="14"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="O15" s="4">
+        <v>710.73203000000001</v>
+      </c>
+      <c r="P15" s="4">
+        <v>335.60883000000001</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>13.548</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15" s="4">
+        <v>1059.88886</v>
+      </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
@@ -6189,14 +6259,28 @@
       <c r="J16" s="16"/>
       <c r="K16" s="14"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
+      <c r="O16" s="4">
+        <v>1592.901827801438</v>
+      </c>
+      <c r="P16" s="4">
+        <v>46.285925000000006</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>26.986585121249998</v>
+      </c>
+      <c r="R16" s="4">
+        <v>28.360250000000001</v>
+      </c>
+      <c r="S16" s="4">
+        <v>9.9607500000000009</v>
+      </c>
+      <c r="T16" s="4">
+        <v>1704.4953379226879</v>
+      </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
@@ -6453,14 +6537,28 @@
       <c r="J17" s="3"/>
       <c r="K17" s="14"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
+      <c r="O17" s="4">
+        <v>7.9033390978040003</v>
+      </c>
+      <c r="P17" s="4">
+        <v>6.7634080000000001</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>3.8740000000000001</v>
+      </c>
+      <c r="R17" s="4">
+        <v>1.7284000000000002</v>
+      </c>
+      <c r="S17" s="4">
+        <v>1.1741199999999998</v>
+      </c>
+      <c r="T17" s="4">
+        <v>21.443267097804</v>
+      </c>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
@@ -6697,14 +6795,28 @@
       <c r="J18" s="3"/>
       <c r="K18" s="14"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="O18" s="4">
+        <v>8440.6803619294606</v>
+      </c>
+      <c r="P18" s="4">
+        <v>3605.3150430000001</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1137.9361982912501</v>
+      </c>
+      <c r="R18" s="4">
+        <v>2133.6398300000005</v>
+      </c>
+      <c r="S18" s="4">
+        <v>696.50317000000007</v>
+      </c>
+      <c r="T18" s="4">
+        <v>16014.07460322071</v>
+      </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
@@ -7205,14 +7317,28 @@
       <c r="J20" s="3"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="O20" s="4">
+        <v>18.958874153611692</v>
+      </c>
+      <c r="P20" s="4">
+        <v>56.309847889544507</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>14.155931772886333</v>
+      </c>
+      <c r="R20" s="4">
+        <v>25.843505692829464</v>
+      </c>
+      <c r="S20" s="4">
+        <v>43.26106645962733</v>
+      </c>
+      <c r="T20" s="4">
+        <v>23.26672817921397</v>
+      </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
@@ -7713,14 +7839,28 @@
       <c r="J22" s="3"/>
       <c r="K22" s="14"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
+      <c r="O22" s="4">
+        <v>15972.450569727</v>
+      </c>
+      <c r="P22" s="4">
+        <v>238.91200000000001</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>600.09470903299996</v>
+      </c>
+      <c r="R22" s="4">
+        <v>665.71</v>
+      </c>
+      <c r="S22" s="4">
+        <v>380.8</v>
+      </c>
+      <c r="T22" s="4">
+        <v>17857.967278759999</v>
+      </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
@@ -8223,7 +8363,9 @@
       <c r="J24" s="16"/>
       <c r="K24" s="26"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -8487,14 +8629,28 @@
       <c r="J25" s="16"/>
       <c r="K25" s="14"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
+      <c r="M25" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
+      <c r="O25" s="4">
+        <v>94256.845479921001</v>
+      </c>
+      <c r="P25" s="4">
+        <v>534.73397999999997</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>3533.33012328</v>
+      </c>
+      <c r="R25" s="4">
+        <v>77.12</v>
+      </c>
+      <c r="S25" s="4">
+        <v>105.59</v>
+      </c>
+      <c r="T25" s="4">
+        <v>98507.619583200998</v>
+      </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
@@ -8751,14 +8907,28 @@
       <c r="J26" s="16"/>
       <c r="K26" s="14"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
+      <c r="O26" s="4">
+        <v>42846.268449704003</v>
+      </c>
+      <c r="P26" s="4">
+        <v>2085.8160600000001</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>1932.696238665</v>
+      </c>
+      <c r="R26" s="4">
+        <v>1193.19</v>
+      </c>
+      <c r="S26" s="4">
+        <v>469.8</v>
+      </c>
+      <c r="T26" s="4">
+        <v>48527.770748369003</v>
+      </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
@@ -9015,14 +9185,28 @@
       <c r="J27" s="16"/>
       <c r="K27" s="14"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
+      <c r="O27" s="4">
+        <v>1548.1094865510001</v>
+      </c>
+      <c r="P27" s="4">
+        <v>929.76693999999998</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>120.18351857499999</v>
+      </c>
+      <c r="R27" s="4">
+        <v>14.73</v>
+      </c>
+      <c r="S27" s="4">
+        <v>88.02000000000001</v>
+      </c>
+      <c r="T27" s="4">
+        <v>2700.809945126</v>
+      </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
@@ -9259,14 +9443,28 @@
       <c r="J28" s="3"/>
       <c r="K28" s="14"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
+      <c r="O28" s="4">
+        <v>1246.1935030069999</v>
+      </c>
+      <c r="P28" s="4">
+        <v>114.93527</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>78.333718743999995</v>
+      </c>
+      <c r="R28" s="4">
+        <v>52</v>
+      </c>
+      <c r="S28" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="T28" s="4">
+        <v>1507.8624917509999</v>
+      </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
@@ -9768,7 +9966,9 @@
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="14"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -10030,14 +10230,28 @@
       <c r="J31" s="3"/>
       <c r="K31" s="14"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
+      <c r="O31" s="4">
+        <v>81.33</v>
+      </c>
+      <c r="P31" s="4">
+        <v>58.277000000000001</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>16.857970160000001</v>
+      </c>
+      <c r="R31" s="4">
+        <v>38.119999999999997</v>
+      </c>
+      <c r="S31" s="4">
+        <v>4.165</v>
+      </c>
+      <c r="T31" s="4">
+        <v>198.74997016</v>
+      </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
@@ -10294,14 +10508,28 @@
       <c r="J32" s="3"/>
       <c r="K32" s="14"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
+      <c r="O32" s="4">
+        <v>5.6031334342578987</v>
+      </c>
+      <c r="P32" s="4">
+        <v>1.7892880000319999</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R32" s="4">
+        <v>0</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T32" s="4">
+        <v>7.3924214342898988</v>
+      </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
@@ -10538,14 +10766,28 @@
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
+      <c r="O33" s="4">
+        <v>86.933133434257897</v>
+      </c>
+      <c r="P33" s="4">
+        <v>60.066288000032003</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>16.857970160000001</v>
+      </c>
+      <c r="R33" s="4">
+        <v>38.119999999999997</v>
+      </c>
+      <c r="S33" s="4">
+        <v>4.165</v>
+      </c>
+      <c r="T33" s="4">
+        <v>206.1423915942899</v>
+      </c>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
@@ -11028,7 +11270,9 @@
       <c r="J35" s="9"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
@@ -11534,7 +11778,9 @@
       <c r="J37" s="3"/>
       <c r="K37" s="14"/>
       <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
+      <c r="M37" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
@@ -11798,14 +12044,28 @@
       <c r="J38" s="3"/>
       <c r="K38" s="14"/>
       <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
+      <c r="M38" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
+      <c r="O38" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="P38" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>1.6238950000000001</v>
+      </c>
+      <c r="R38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S38" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="T38" s="4">
+        <v>9.2238950000000006</v>
+      </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
@@ -12062,14 +12322,28 @@
       <c r="J39" s="3"/>
       <c r="K39" s="14"/>
       <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
+      <c r="M39" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
+      <c r="O39" s="4">
+        <v>26.665239999999997</v>
+      </c>
+      <c r="P39" s="4">
+        <v>0.11321200000000001</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>25.853999999999999</v>
+      </c>
+      <c r="R39" s="4">
+        <v>0</v>
+      </c>
+      <c r="S39" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="T39" s="4">
+        <v>52.633552000000002</v>
+      </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
@@ -12326,14 +12600,28 @@
       <c r="J40" s="3"/>
       <c r="K40" s="14"/>
       <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
+      <c r="M40" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="N40" s="13"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
+      <c r="O40" s="4">
+        <v>49.61356</v>
+      </c>
+      <c r="P40" s="4">
+        <v>24.410564999999998</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>0</v>
+      </c>
+      <c r="R40" s="4">
+        <v>0</v>
+      </c>
+      <c r="S40" s="4">
+        <v>0</v>
+      </c>
+      <c r="T40" s="4">
+        <v>74.024124999999998</v>
+      </c>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
@@ -12570,14 +12858,28 @@
       <c r="J41" s="3"/>
       <c r="K41" s="14"/>
       <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
+      <c r="M41" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
+      <c r="O41" s="4">
+        <v>0</v>
+      </c>
+      <c r="P41" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>129.48417890000002</v>
+      </c>
+      <c r="R41" s="4">
+        <v>0</v>
+      </c>
+      <c r="S41" s="4">
+        <v>0</v>
+      </c>
+      <c r="T41" s="4">
+        <v>129.48417890000002</v>
+      </c>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
@@ -13075,7 +13377,9 @@
       <c r="J43" s="16"/>
       <c r="K43" s="14"/>
       <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
+      <c r="M43" s="18" t="s">
+        <v>17</v>
+      </c>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
@@ -13334,14 +13638,28 @@
       <c r="J44" s="16"/>
       <c r="K44" s="14"/>
       <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
+      <c r="M44" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
+      <c r="O44" s="4">
+        <v>1</v>
+      </c>
+      <c r="P44" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>0</v>
+      </c>
+      <c r="R44" s="4">
+        <v>0</v>
+      </c>
+      <c r="S44" s="4">
+        <v>0</v>
+      </c>
+      <c r="T44" s="4">
+        <v>2</v>
+      </c>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
@@ -13593,14 +13911,28 @@
       <c r="J45" s="16"/>
       <c r="K45" s="14"/>
       <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
+      <c r="M45" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
+      <c r="O45" s="4">
+        <v>195</v>
+      </c>
+      <c r="P45" s="4">
+        <v>104</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>0</v>
+      </c>
+      <c r="R45" s="4">
+        <v>0</v>
+      </c>
+      <c r="S45" s="4">
+        <v>0</v>
+      </c>
+      <c r="T45" s="4">
+        <v>299</v>
+      </c>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
@@ -13852,14 +14184,28 @@
       <c r="J46" s="16"/>
       <c r="K46" s="14"/>
       <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
+      <c r="M46" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
+      <c r="O46" s="4">
+        <v>96</v>
+      </c>
+      <c r="P46" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>0</v>
+      </c>
+      <c r="R46" s="4">
+        <v>0</v>
+      </c>
+      <c r="S46" s="4">
+        <v>0</v>
+      </c>
+      <c r="T46" s="4">
+        <v>99</v>
+      </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
@@ -14111,14 +14457,28 @@
       <c r="J47" s="16"/>
       <c r="K47" s="14"/>
       <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
+      <c r="M47" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
+      <c r="O47" s="4">
+        <v>749</v>
+      </c>
+      <c r="P47" s="4">
+        <v>112</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>0</v>
+      </c>
+      <c r="R47" s="4">
+        <v>0</v>
+      </c>
+      <c r="S47" s="4">
+        <v>0</v>
+      </c>
+      <c r="T47" s="4">
+        <v>861</v>
+      </c>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
@@ -14355,14 +14715,28 @@
       <c r="J48" s="16"/>
       <c r="K48" s="14"/>
       <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
+      <c r="M48" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
+      <c r="O48" s="4">
+        <v>390</v>
+      </c>
+      <c r="P48" s="4">
+        <v>106</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>0</v>
+      </c>
+      <c r="R48" s="4">
+        <v>0</v>
+      </c>
+      <c r="S48" s="4">
+        <v>0</v>
+      </c>
+      <c r="T48" s="4">
+        <v>496</v>
+      </c>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
@@ -14865,7 +15239,9 @@
       <c r="J50" s="16"/>
       <c r="K50" s="14"/>
       <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
+      <c r="M50" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
@@ -15129,14 +15505,28 @@
       <c r="J51" s="16"/>
       <c r="K51" s="14"/>
       <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
+      <c r="M51" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
+      <c r="O51" s="4">
+        <v>23.32</v>
+      </c>
+      <c r="P51" s="4">
+        <v>69791</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>8540.1005999999998</v>
+      </c>
+      <c r="R51" s="4">
+        <v>4.42</v>
+      </c>
+      <c r="S51" s="4">
+        <v>240.92</v>
+      </c>
+      <c r="T51" s="4">
+        <v>78599.760600000009</v>
+      </c>
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
@@ -15393,14 +15783,28 @@
       <c r="J52" s="16"/>
       <c r="K52" s="14"/>
       <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
+      <c r="M52" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
+      <c r="O52" s="4">
+        <v>197546.25</v>
+      </c>
+      <c r="P52" s="4">
+        <v>121554</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>3114.5836600000002</v>
+      </c>
+      <c r="R52" s="4">
+        <v>144.52000000000001</v>
+      </c>
+      <c r="S52" s="4">
+        <v>129.26300000000001</v>
+      </c>
+      <c r="T52" s="4">
+        <v>322488.61666</v>
+      </c>
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
       <c r="W52" s="4"/>
@@ -15657,14 +16061,28 @@
       <c r="J53" s="3"/>
       <c r="K53" s="14"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
+      <c r="O53" s="4">
+        <v>252483.16</v>
+      </c>
+      <c r="P53" s="4">
+        <v>5311</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>7168.9109500000004</v>
+      </c>
+      <c r="R53" s="4">
+        <v>518.64</v>
+      </c>
+      <c r="S53" s="4">
+        <v>25.83</v>
+      </c>
+      <c r="T53" s="4">
+        <v>265507.54095000005</v>
+      </c>
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
@@ -15921,14 +16339,28 @@
       <c r="J54" s="3"/>
       <c r="K54" s="14"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
+      <c r="O54" s="4">
+        <v>450052.73</v>
+      </c>
+      <c r="P54" s="4">
+        <v>196656</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>18823.595209999999</v>
+      </c>
+      <c r="R54" s="4">
+        <v>667.57999999999993</v>
+      </c>
+      <c r="S54" s="4">
+        <v>396.01299999999998</v>
+      </c>
+      <c r="T54" s="4">
+        <v>666595.91821000003</v>
+      </c>
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
       <c r="W54" s="4"/>
@@ -16165,14 +16597,28 @@
       <c r="J55" s="3"/>
       <c r="K55" s="14"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
+      <c r="M55" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
+      <c r="O55" s="4">
+        <v>197569.57</v>
+      </c>
+      <c r="P55" s="4">
+        <v>191345</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>11654.68426</v>
+      </c>
+      <c r="R55" s="4">
+        <v>148.94</v>
+      </c>
+      <c r="S55" s="4">
+        <v>370.18299999999999</v>
+      </c>
+      <c r="T55" s="4">
+        <v>401088.37725999998</v>
+      </c>
       <c r="U55" s="4"/>
       <c r="V55" s="4"/>
       <c r="W55" s="4"/>
@@ -16899,7 +17345,9 @@
       <c r="J58" s="3"/>
       <c r="K58" s="14"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
+      <c r="M58" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
       <c r="P58" s="4"/>
@@ -17427,14 +17875,28 @@
       <c r="J60" s="3"/>
       <c r="K60" s="14"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
+      <c r="M60" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
+      <c r="O60" s="4">
+        <v>6240</v>
+      </c>
+      <c r="P60" s="4">
+        <v>820</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>1940</v>
+      </c>
+      <c r="R60" s="4">
+        <v>300</v>
+      </c>
+      <c r="S60" s="4">
+        <v>230</v>
+      </c>
+      <c r="T60" s="4">
+        <v>9500</v>
+      </c>
       <c r="U60" s="4"/>
       <c r="V60" s="4"/>
       <c r="W60" s="4"/>
@@ -17691,14 +18153,28 @@
       <c r="J61" s="3"/>
       <c r="K61" s="14"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
+      <c r="M61" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
+      <c r="O61" s="4">
+        <v>0.28788849727651394</v>
+      </c>
+      <c r="P61" s="4">
+        <v>0.25766871165644173</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>0.21039094650205761</v>
+      </c>
+      <c r="R61" s="4">
+        <v>0.19256756756756757</v>
+      </c>
+      <c r="S61" s="4">
+        <v>0.4933920704845815</v>
+      </c>
+      <c r="T61" s="4">
+        <v>0.27100000000000002</v>
+      </c>
       <c r="U61" s="4"/>
       <c r="V61" s="4"/>
       <c r="W61" s="4"/>
@@ -17955,14 +18431,28 @@
       <c r="J62" s="3"/>
       <c r="K62" s="14"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
+      <c r="M62" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
+      <c r="O62" s="4">
+        <v>0.26476190476190475</v>
+      </c>
+      <c r="P62" s="4">
+        <v>0.26282051282051283</v>
+      </c>
+      <c r="Q62" s="4">
+        <v>0.22968197879858657</v>
+      </c>
+      <c r="R62" s="4">
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="S62" s="4">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="T62" s="4">
+        <v>0.26</v>
+      </c>
       <c r="U62" s="4"/>
       <c r="V62" s="4"/>
       <c r="W62" s="4"/>
@@ -18219,14 +18709,28 @@
       <c r="J63" s="3"/>
       <c r="K63" s="14"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
+      <c r="M63" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
+      <c r="O63" s="4">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="P63" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="R63" s="4">
+        <v>0</v>
+      </c>
+      <c r="S63" s="4">
+        <v>0</v>
+      </c>
+      <c r="T63" s="4">
+        <v>0.25</v>
+      </c>
       <c r="U63" s="4"/>
       <c r="V63" s="4"/>
       <c r="W63" s="4"/>
@@ -18483,14 +18987,28 @@
       <c r="J64" s="3"/>
       <c r="K64" s="14"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
+      <c r="M64" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-      <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
+      <c r="O64" s="4">
+        <v>0.26237623762376239</v>
+      </c>
+      <c r="P64" s="4">
+        <v>0.26950354609929078</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="R64" s="4">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="S64" s="4">
+        <v>0.46511627906976744</v>
+      </c>
+      <c r="T64" s="4">
+        <v>0.26</v>
+      </c>
       <c r="U64" s="4"/>
       <c r="V64" s="4"/>
       <c r="W64" s="4"/>
@@ -18747,14 +19265,28 @@
       <c r="J65" s="3"/>
       <c r="K65" s="14"/>
       <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
+      <c r="M65" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
+      <c r="O65" s="4">
+        <v>0.31093716025222873</v>
+      </c>
+      <c r="P65" s="4">
+        <v>0.31419457735247208</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>0.27150749802683505</v>
+      </c>
+      <c r="R65" s="4">
+        <v>0.1672473867595819</v>
+      </c>
+      <c r="S65" s="4">
+        <v>0.4719626168224299</v>
+      </c>
+      <c r="T65" s="4">
+        <v>0.3031169573920503</v>
+      </c>
       <c r="U65" s="4"/>
       <c r="V65" s="4"/>
       <c r="W65" s="4"/>
@@ -19011,14 +19543,28 @@
       <c r="J66" s="3"/>
       <c r="K66" s="14"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
+      <c r="M66" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
+      <c r="O66" s="4">
+        <v>0.2012072434607646</v>
+      </c>
+      <c r="P66" s="4">
+        <v>0.20100502512562815</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>0.24669603524229075</v>
+      </c>
+      <c r="R66" s="4">
+        <v>0.18867924528301888</v>
+      </c>
+      <c r="S66" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="T66" s="4">
+        <v>0.21134249003101463</v>
+      </c>
       <c r="U66" s="4"/>
       <c r="V66" s="4"/>
       <c r="W66" s="4"/>
@@ -19275,14 +19821,28 @@
       <c r="J67" s="3"/>
       <c r="K67" s="14"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
+      <c r="M67" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
+      <c r="O67" s="4">
+        <v>10.11823133611022</v>
+      </c>
+      <c r="P67" s="4">
+        <v>9.3509202453987736</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>14.382716049382717</v>
+      </c>
+      <c r="R67" s="4">
+        <v>7.8952702702702702</v>
+      </c>
+      <c r="S67" s="4">
+        <v>10.775330396475772</v>
+      </c>
+      <c r="T67" s="4">
+        <v>10.9</v>
+      </c>
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
       <c r="W67" s="4"/>
@@ -19521,14 +20081,28 @@
       <c r="J68" s="3"/>
       <c r="K68" s="14"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
+      <c r="M68" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
+      <c r="O68" s="4">
+        <v>16.19352771547581</v>
+      </c>
+      <c r="P68" s="4">
+        <v>18.736196319018404</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>20.760288065843621</v>
+      </c>
+      <c r="R68" s="4">
+        <v>19.631756756756758</v>
+      </c>
+      <c r="S68" s="4">
+        <v>18.58590308370044</v>
+      </c>
+      <c r="T68" s="4">
+        <v>17.5</v>
+      </c>
       <c r="U68" s="4"/>
       <c r="V68" s="4"/>
       <c r="W68" s="4"/>
@@ -19785,7 +20359,9 @@
       <c r="J69" s="3"/>
       <c r="K69" s="14"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
+      <c r="M69" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
       <c r="P69" s="4"/>
@@ -20049,14 +20625,28 @@
       <c r="J70" s="3"/>
       <c r="K70" s="14"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
+      <c r="M70" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
+      <c r="O70" s="4">
+        <v>0.10781800704902275</v>
+      </c>
+      <c r="P70" s="4">
+        <v>3.6809815950920248E-2</v>
+      </c>
+      <c r="Q70" s="4">
+        <v>8.5390946502057613E-2</v>
+      </c>
+      <c r="R70" s="4">
+        <v>5.4054054054054057E-2</v>
+      </c>
+      <c r="S70" s="4">
+        <v>1.7621145374449341E-2</v>
+      </c>
+      <c r="T70" s="4">
+        <v>7.5999999999999998E-2</v>
+      </c>
       <c r="U70" s="4"/>
       <c r="V70" s="4"/>
       <c r="W70" s="4"/>
@@ -20313,14 +20903,28 @@
       <c r="J71" s="3"/>
       <c r="K71" s="14"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
+      <c r="M71" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-      <c r="S71" s="4"/>
-      <c r="T71" s="4"/>
+      <c r="O71" s="4">
+        <v>0.6054149311118231</v>
+      </c>
+      <c r="P71" s="4">
+        <v>0.72883435582822087</v>
+      </c>
+      <c r="Q71" s="4">
+        <v>0.50617283950617287</v>
+      </c>
+      <c r="R71" s="4">
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="S71" s="4">
+        <v>0.76211453744493396</v>
+      </c>
+      <c r="T71" s="4">
+        <v>0.61899999999999999</v>
+      </c>
       <c r="U71" s="4"/>
       <c r="V71" s="4"/>
       <c r="W71" s="4"/>
@@ -20557,14 +21161,28 @@
       <c r="J72" s="3"/>
       <c r="K72" s="14"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
+      <c r="M72" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
-      <c r="Q72" s="4"/>
-      <c r="R72" s="4"/>
-      <c r="S72" s="4"/>
-      <c r="T72" s="4"/>
+      <c r="O72" s="4">
+        <v>0.28676706183915412</v>
+      </c>
+      <c r="P72" s="4">
+        <v>0.2343558282208589</v>
+      </c>
+      <c r="Q72" s="4">
+        <v>0.40843621399176955</v>
+      </c>
+      <c r="R72" s="4">
+        <v>0.27027027027027029</v>
+      </c>
+      <c r="S72" s="4">
+        <v>0.22026431718061673</v>
+      </c>
+      <c r="T72" s="4">
+        <v>0.30499999999999999</v>
+      </c>
       <c r="U72" s="4"/>
       <c r="V72" s="4"/>
       <c r="W72" s="4"/>
@@ -21291,7 +21909,9 @@
       <c r="J75" s="3"/>
       <c r="K75" s="14"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
+      <c r="M75" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
@@ -21799,14 +22419,28 @@
       <c r="J77" s="3"/>
       <c r="K77" s="14"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
+      <c r="M77" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
-      <c r="S77" s="4"/>
-      <c r="T77" s="4"/>
+      <c r="O77" s="4">
+        <v>445.21</v>
+      </c>
+      <c r="P77" s="4">
+        <v>64.026368000000005</v>
+      </c>
+      <c r="Q77" s="4">
+        <v>80.385821050000004</v>
+      </c>
+      <c r="R77" s="4">
+        <v>82.56</v>
+      </c>
+      <c r="S77" s="4">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="T77" s="4">
+        <v>688.28218905000006</v>
+      </c>
       <c r="U77" s="4"/>
       <c r="V77" s="4"/>
       <c r="W77" s="4"/>
@@ -25281,12 +25915,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25543,22 +26181,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
+    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
+    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25585,20 +26230,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
-    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
-    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed Data.xlsx to put certain info into different tabs
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
+++ b/Data Sets (Excels)/detailed-metrics-chart-by-country-6-15-23-2.xlsx
@@ -2112,6 +2112,10 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2414,8 +2418,8 @@
   </sheetPr>
   <dimension ref="A1:IH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -25915,19 +25919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005230FC7721ADAB429BE220CF608D2E9F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c69ef8cf067ed40c1830b4bee094226f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b5c83d36-6b3e-42ba-8ee3-100325a63de4" xmlns:ns3="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3" xmlns:ns4="b2489833-8b1e-44ca-badd-e803b46be494" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78be28c9ca3bdb29dba3cd8e3c26ea70" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -26180,6 +26171,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b2489833-8b1e-44ca-badd-e803b46be494" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5c83d36-6b3e-42ba-8ee3-100325a63de4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -26190,25 +26194,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
-    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
-    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9777DCF-02F2-4A82-A34F-41E92F786BE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26229,6 +26214,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA43A20-A029-4183-9CDB-556B30DC3D1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b2489833-8b1e-44ca-badd-e803b46be494"/>
+    <ds:schemaRef ds:uri="9fc062f7-da3d-45c0-bbaa-e183b1ca8cd3"/>
+    <ds:schemaRef ds:uri="b5c83d36-6b3e-42ba-8ee3-100325a63de4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E834397F-6075-4609-8B75-21CCD0A4812E}">
   <ds:schemaRefs>

</xml_diff>